<commit_message>
Updated estimation excel sheet
</commit_message>
<xml_diff>
--- a/Files/Requirement/Time Estimation.xlsx
+++ b/Files/Requirement/Time Estimation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Id</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -516,7 +519,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -563,7 +566,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45">

</xml_diff>

<commit_message>
updated time estimation worksheet
</commit_message>
<xml_diff>
--- a/Files/Requirement/Time Estimation.xlsx
+++ b/Files/Requirement/Time Estimation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Id</t>
   </si>
@@ -58,12 +58,6 @@
   </si>
   <si>
     <t>Additional Tasks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  a. Implement the scene loader with transition logic
-  b. Setup the camera with a fader
-  c. Integrate and test the fader
-</t>
   </si>
   <si>
     <t xml:space="preserve">  a. Create a JSON structure and equivalent model classes for storing the quotes
@@ -132,6 +126,19 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  a. Add loading HUD
+  b. Implement the scene loader with transition logic
+  c. Setup the camera with a fader
+d. Integrate and test the fader
+</t>
+  </si>
+  <si>
+    <t>* Createdd Loading Curosr HUD prefab with spinnng animation</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -201,14 +208,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -218,6 +221,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,7 +528,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -529,52 +541,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60">
+    <row r="2" spans="1:6" ht="75">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D2" s="3">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F2" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D3" s="3">
         <v>2</v>
@@ -588,11 +602,11 @@
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D4" s="3">
         <v>3</v>
@@ -606,11 +620,11 @@
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -624,11 +638,11 @@
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
+      <c r="C6" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>2</v>
@@ -642,11 +656,11 @@
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>19</v>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -660,11 +674,11 @@
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>20</v>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D8" s="3">
         <v>4</v>
@@ -675,17 +689,20 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="C9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9">
-        <f>SUM(D2:D8)</f>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="7">
         <v>20</v>
       </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="30">
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hud display handler update
</commit_message>
<xml_diff>
--- a/Files/Requirement/Time Estimation.xlsx
+++ b/Files/Requirement/Time Estimation.xlsx
@@ -68,20 +68,6 @@
     <t xml:space="preserve">  a. Create the progress bar logic
   b. Create UI for progress bar
   c. Integrate progress bar with scene loader to update the delay
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Scene Transition Process flow
-   § User enters the entry scene. 
-   § Entry scene waits for a user input to start loading the main scene
-   § As the main scene starts to load, the fader fades to black and rand quote text and progress bar appears
-   § When the loading complete the camera fades out to the main scene
-  a. Create the entry scene
-  b. Create UI for main scene loading
-  c. Integrate fader and progress bar functionalities to work together
-  d. Setup camera culling to certain layers so that artifacts from entry scene are invisible while the scene loads
-  e. Introduce a simulated delay to  demonstrate the random quotes
-  f. Add a free unity environment asset as the main scene and setup basic teleport navigation in the scene
 </t>
   </si>
   <si>
@@ -128,17 +114,31 @@
     <t>Total</t>
   </si>
   <si>
+    <t>* Createdd Loading Curosr HUD prefab with spinnng animation</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
     <t xml:space="preserve">  a. Add loading HUD
-  b. Implement the scene loader with transition logic
-  c. Setup the camera with a fader
-d. Integrate and test the fader
 </t>
   </si>
   <si>
-    <t>* Createdd Loading Curosr HUD prefab with spinnng animation</t>
-  </si>
-  <si>
-    <t>In progress</t>
+    <t xml:space="preserve"> Scene Transition Process flow
+   § User enters the entry scene. 
+   § Entry scene waits for a user input to start loading the main scene
+   § As the main scene starts to load, the fader fades to black and rand quote text and progress bar appears
+   § When the loading complete the camera fades out to the main scene
+  a. Implement the scene loader with transition logic
+  b. Setup the camera with a fader
+  c. Integrate and test the fader
+  d. Create the entry scene
+  e. Create UI for main scene loading
+  f. Integrate fader and progress bar functionalities to work together
+  g. Setup camera culling to certain layers so that artifacts from entry scene are invisible while the scene loads
+  h. Introduce a simulated delay to  demonstrate the random quotes
+  i. Add a free unity environment asset as the main scene and setup basic teleport navigation in the scene
+</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -568,16 +568,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="3">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45">
@@ -616,7 +616,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="240">
+    <row r="5" spans="1:6" ht="285">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -624,14 +624,14 @@
         <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45">
@@ -642,7 +642,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3">
         <v>2</v>
@@ -660,7 +660,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -678,7 +678,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3">
         <v>4</v>
@@ -692,7 +692,7 @@
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="7">
         <v>20</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="11" spans="1:6" ht="30">
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>